<commit_message>
Import de données OK
</commit_message>
<xml_diff>
--- a/src/main/resources/file/liste-patient-symptome.xlsx
+++ b/src/main/resources/file/liste-patient-symptome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nomena/S5/Mr-Tahina/Docteur/src/main/resources/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BBCE58-37F2-FA49-973B-4BECADFB7186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BE1D7-AF89-8643-891D-03E07AB84D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{D97048E4-30E5-794B-A2C6-A877D153CFE1}"/>
   </bookViews>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF35D1-C5DA-B642-AD5D-DCCBCD7CBC77}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,9 +451,25 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bref, ça marche !
</commit_message>
<xml_diff>
--- a/src/main/resources/file/liste-patient-symptome.xlsx
+++ b/src/main/resources/file/liste-patient-symptome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nomena/S5/Mr-Tahina/Docteur/src/main/resources/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1BE1D7-AF89-8643-891D-03E07AB84D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4975D238-5361-A04F-AA64-2813DFCA1D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{D97048E4-30E5-794B-A2C6-A877D153CFE1}"/>
   </bookViews>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF35D1-C5DA-B642-AD5D-DCCBCD7CBC77}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,25 +451,9 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
         <v>9</v>
       </c>
     </row>

</xml_diff>